<commit_message>
Add a comment extension on the CarePlan.participant
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-anticipate-directives-exist.xlsx
+++ b/output/StructureDefinition-anticipate-directives-exist.xlsx
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Existence of AD</t>
+    <t>Existence of Advance Directives</t>
   </si>
   <si>
     <t>Status</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-18T14:12:38+02:00</t>
+    <t>2023-07-18T14:23:59+02:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>